<commit_message>
Latest versions of datasets
</commit_message>
<xml_diff>
--- a/bax_insertion/data/KD3_dataset.xlsx
+++ b/bax_insertion/data/KD3_dataset.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="12330"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="27795" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Dataset" sheetId="1" r:id="rId1"/>
+    <sheet name="Endpoints" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="11">
   <si>
     <t>cBid</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>Activator:</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>STDEV</t>
+  </si>
+  <si>
+    <t>RLS</t>
   </si>
 </sst>
 </file>
@@ -594,6 +603,9 @@
     <xf numFmtId="0" fontId="1" fillId="18" borderId="13" xfId="27" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="27" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="18"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="10" xfId="18" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -618,9 +630,6 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="12" xfId="28" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="18"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -965,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DE138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,469 +984,469 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:109" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="8">
         <v>3</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="5">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="8">
         <v>36</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="5">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="8">
         <v>54</v>
       </c>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AD1" s="6"/>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="6"/>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="6"/>
-      <c r="AL1" s="5">
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="8">
         <v>68</v>
       </c>
-      <c r="AM1" s="6"/>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="6"/>
-      <c r="AP1" s="6"/>
-      <c r="AQ1" s="6"/>
-      <c r="AR1" s="6"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="6"/>
-      <c r="AV1" s="6"/>
-      <c r="AW1" s="6"/>
-      <c r="AX1" s="5">
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="9"/>
+      <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
+      <c r="AX1" s="8">
         <v>120</v>
       </c>
-      <c r="AY1" s="6"/>
-      <c r="AZ1" s="6"/>
-      <c r="BA1" s="6"/>
-      <c r="BB1" s="6"/>
-      <c r="BC1" s="6"/>
-      <c r="BD1" s="6"/>
-      <c r="BE1" s="6"/>
-      <c r="BF1" s="6"/>
-      <c r="BG1" s="6"/>
-      <c r="BH1" s="6"/>
-      <c r="BI1" s="6"/>
-      <c r="BJ1" s="5">
+      <c r="AY1" s="9"/>
+      <c r="AZ1" s="9"/>
+      <c r="BA1" s="9"/>
+      <c r="BB1" s="9"/>
+      <c r="BC1" s="9"/>
+      <c r="BD1" s="9"/>
+      <c r="BE1" s="9"/>
+      <c r="BF1" s="9"/>
+      <c r="BG1" s="9"/>
+      <c r="BH1" s="9"/>
+      <c r="BI1" s="9"/>
+      <c r="BJ1" s="8">
         <v>126</v>
       </c>
-      <c r="BK1" s="6"/>
-      <c r="BL1" s="6"/>
-      <c r="BM1" s="6"/>
-      <c r="BN1" s="6"/>
-      <c r="BO1" s="6"/>
-      <c r="BP1" s="6"/>
-      <c r="BQ1" s="6"/>
-      <c r="BR1" s="6"/>
-      <c r="BS1" s="6"/>
-      <c r="BT1" s="6"/>
-      <c r="BU1" s="6"/>
-      <c r="BV1" s="5">
+      <c r="BK1" s="9"/>
+      <c r="BL1" s="9"/>
+      <c r="BM1" s="9"/>
+      <c r="BN1" s="9"/>
+      <c r="BO1" s="9"/>
+      <c r="BP1" s="9"/>
+      <c r="BQ1" s="9"/>
+      <c r="BR1" s="9"/>
+      <c r="BS1" s="9"/>
+      <c r="BT1" s="9"/>
+      <c r="BU1" s="9"/>
+      <c r="BV1" s="8">
         <v>138</v>
       </c>
-      <c r="BW1" s="6"/>
-      <c r="BX1" s="6"/>
-      <c r="BY1" s="6"/>
-      <c r="BZ1" s="6"/>
-      <c r="CA1" s="6"/>
-      <c r="CB1" s="6"/>
-      <c r="CC1" s="6"/>
-      <c r="CD1" s="6"/>
-      <c r="CE1" s="6"/>
-      <c r="CF1" s="6"/>
-      <c r="CG1" s="6"/>
-      <c r="CH1" s="5">
+      <c r="BW1" s="9"/>
+      <c r="BX1" s="9"/>
+      <c r="BY1" s="9"/>
+      <c r="BZ1" s="9"/>
+      <c r="CA1" s="9"/>
+      <c r="CB1" s="9"/>
+      <c r="CC1" s="9"/>
+      <c r="CD1" s="9"/>
+      <c r="CE1" s="9"/>
+      <c r="CF1" s="9"/>
+      <c r="CG1" s="9"/>
+      <c r="CH1" s="8">
         <v>175</v>
       </c>
-      <c r="CI1" s="6"/>
-      <c r="CJ1" s="6"/>
-      <c r="CK1" s="6"/>
-      <c r="CL1" s="6"/>
-      <c r="CM1" s="6"/>
-      <c r="CN1" s="6"/>
-      <c r="CO1" s="6"/>
-      <c r="CP1" s="6"/>
-      <c r="CQ1" s="6"/>
-      <c r="CR1" s="6"/>
-      <c r="CS1" s="6"/>
-      <c r="CT1" s="5">
+      <c r="CI1" s="9"/>
+      <c r="CJ1" s="9"/>
+      <c r="CK1" s="9"/>
+      <c r="CL1" s="9"/>
+      <c r="CM1" s="9"/>
+      <c r="CN1" s="9"/>
+      <c r="CO1" s="9"/>
+      <c r="CP1" s="9"/>
+      <c r="CQ1" s="9"/>
+      <c r="CR1" s="9"/>
+      <c r="CS1" s="9"/>
+      <c r="CT1" s="8">
         <v>179</v>
       </c>
-      <c r="CU1" s="6"/>
-      <c r="CV1" s="6"/>
-      <c r="CW1" s="6"/>
-      <c r="CX1" s="6"/>
-      <c r="CY1" s="6"/>
-      <c r="CZ1" s="6"/>
-      <c r="DA1" s="6"/>
-      <c r="DB1" s="6"/>
-      <c r="DC1" s="6"/>
-      <c r="DD1" s="6"/>
-      <c r="DE1" s="6"/>
+      <c r="CU1" s="9"/>
+      <c r="CV1" s="9"/>
+      <c r="CW1" s="9"/>
+      <c r="CX1" s="9"/>
+      <c r="CY1" s="9"/>
+      <c r="CZ1" s="9"/>
+      <c r="DA1" s="9"/>
+      <c r="DB1" s="9"/>
+      <c r="DC1" s="9"/>
+      <c r="DD1" s="9"/>
+      <c r="DE1" s="9"/>
     </row>
     <row r="2" spans="1:109" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="10">
         <v>1</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="7">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="10">
         <v>2</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="7">
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="10">
         <v>3</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="7">
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="10">
         <v>1</v>
       </c>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="7">
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="10">
         <v>2</v>
       </c>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="7">
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="10">
         <v>3</v>
       </c>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="9"/>
-      <c r="Z2" s="7">
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="10">
         <v>1</v>
       </c>
-      <c r="AA2" s="8"/>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="8"/>
-      <c r="AD2" s="7">
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="10">
         <v>2</v>
       </c>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="7">
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="10">
         <v>3</v>
       </c>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="7">
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="10">
         <v>1</v>
       </c>
-      <c r="AM2" s="8"/>
-      <c r="AN2" s="8"/>
-      <c r="AO2" s="8"/>
-      <c r="AP2" s="7">
+      <c r="AM2" s="11"/>
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="10">
         <v>2</v>
       </c>
-      <c r="AQ2" s="8"/>
-      <c r="AR2" s="8"/>
-      <c r="AS2" s="9"/>
-      <c r="AT2" s="7">
+      <c r="AQ2" s="11"/>
+      <c r="AR2" s="11"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="10">
         <v>3</v>
       </c>
-      <c r="AU2" s="8"/>
-      <c r="AV2" s="8"/>
-      <c r="AW2" s="9"/>
-      <c r="AX2" s="7">
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="11"/>
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="10">
         <v>1</v>
       </c>
-      <c r="AY2" s="8"/>
-      <c r="AZ2" s="8"/>
-      <c r="BA2" s="8"/>
-      <c r="BB2" s="7">
+      <c r="AY2" s="11"/>
+      <c r="AZ2" s="11"/>
+      <c r="BA2" s="11"/>
+      <c r="BB2" s="10">
         <v>2</v>
       </c>
-      <c r="BC2" s="8"/>
-      <c r="BD2" s="8"/>
-      <c r="BE2" s="9"/>
-      <c r="BF2" s="7">
+      <c r="BC2" s="11"/>
+      <c r="BD2" s="11"/>
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="10">
         <v>3</v>
       </c>
-      <c r="BG2" s="8"/>
-      <c r="BH2" s="8"/>
-      <c r="BI2" s="9"/>
-      <c r="BJ2" s="7">
+      <c r="BG2" s="11"/>
+      <c r="BH2" s="11"/>
+      <c r="BI2" s="12"/>
+      <c r="BJ2" s="10">
         <v>1</v>
       </c>
-      <c r="BK2" s="8"/>
-      <c r="BL2" s="8"/>
-      <c r="BM2" s="8"/>
-      <c r="BN2" s="7">
+      <c r="BK2" s="11"/>
+      <c r="BL2" s="11"/>
+      <c r="BM2" s="11"/>
+      <c r="BN2" s="10">
         <v>2</v>
       </c>
-      <c r="BO2" s="8"/>
-      <c r="BP2" s="8"/>
-      <c r="BQ2" s="9"/>
-      <c r="BR2" s="7">
+      <c r="BO2" s="11"/>
+      <c r="BP2" s="11"/>
+      <c r="BQ2" s="12"/>
+      <c r="BR2" s="10">
         <v>3</v>
       </c>
-      <c r="BS2" s="8"/>
-      <c r="BT2" s="8"/>
-      <c r="BU2" s="9"/>
-      <c r="BV2" s="7">
+      <c r="BS2" s="11"/>
+      <c r="BT2" s="11"/>
+      <c r="BU2" s="12"/>
+      <c r="BV2" s="10">
         <v>1</v>
       </c>
-      <c r="BW2" s="8"/>
-      <c r="BX2" s="8"/>
-      <c r="BY2" s="8"/>
-      <c r="BZ2" s="7">
+      <c r="BW2" s="11"/>
+      <c r="BX2" s="11"/>
+      <c r="BY2" s="11"/>
+      <c r="BZ2" s="10">
         <v>2</v>
       </c>
-      <c r="CA2" s="8"/>
-      <c r="CB2" s="8"/>
-      <c r="CC2" s="9"/>
-      <c r="CD2" s="7">
+      <c r="CA2" s="11"/>
+      <c r="CB2" s="11"/>
+      <c r="CC2" s="12"/>
+      <c r="CD2" s="10">
         <v>3</v>
       </c>
-      <c r="CE2" s="8"/>
-      <c r="CF2" s="8"/>
-      <c r="CG2" s="9"/>
-      <c r="CH2" s="7">
+      <c r="CE2" s="11"/>
+      <c r="CF2" s="11"/>
+      <c r="CG2" s="12"/>
+      <c r="CH2" s="10">
         <v>1</v>
       </c>
-      <c r="CI2" s="8"/>
-      <c r="CJ2" s="8"/>
-      <c r="CK2" s="8"/>
-      <c r="CL2" s="7">
+      <c r="CI2" s="11"/>
+      <c r="CJ2" s="11"/>
+      <c r="CK2" s="11"/>
+      <c r="CL2" s="10">
         <v>2</v>
       </c>
-      <c r="CM2" s="8"/>
-      <c r="CN2" s="8"/>
-      <c r="CO2" s="9"/>
-      <c r="CP2" s="7">
+      <c r="CM2" s="11"/>
+      <c r="CN2" s="11"/>
+      <c r="CO2" s="12"/>
+      <c r="CP2" s="10">
         <v>3</v>
       </c>
-      <c r="CQ2" s="8"/>
-      <c r="CR2" s="8"/>
-      <c r="CS2" s="9"/>
-      <c r="CT2" s="7">
+      <c r="CQ2" s="11"/>
+      <c r="CR2" s="11"/>
+      <c r="CS2" s="12"/>
+      <c r="CT2" s="10">
         <v>1</v>
       </c>
-      <c r="CU2" s="8"/>
-      <c r="CV2" s="8"/>
-      <c r="CW2" s="8"/>
-      <c r="CX2" s="7">
+      <c r="CU2" s="11"/>
+      <c r="CV2" s="11"/>
+      <c r="CW2" s="11"/>
+      <c r="CX2" s="10">
         <v>2</v>
       </c>
-      <c r="CY2" s="8"/>
-      <c r="CZ2" s="8"/>
-      <c r="DA2" s="9"/>
-      <c r="DB2" s="7">
+      <c r="CY2" s="11"/>
+      <c r="CZ2" s="11"/>
+      <c r="DA2" s="12"/>
+      <c r="DB2" s="10">
         <v>3</v>
       </c>
-      <c r="DC2" s="8"/>
-      <c r="DD2" s="8"/>
-      <c r="DE2" s="9"/>
+      <c r="DC2" s="11"/>
+      <c r="DD2" s="11"/>
+      <c r="DE2" s="12"/>
     </row>
     <row r="3" spans="1:109" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="10" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="10" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="10" t="s">
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="10" t="s">
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="10" t="s">
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="10" t="s">
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-      <c r="AC3" s="12"/>
-      <c r="AD3" s="10" t="s">
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="15"/>
+      <c r="AD3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="AE3" s="11"/>
-      <c r="AF3" s="11"/>
-      <c r="AG3" s="12"/>
-      <c r="AH3" s="10" t="s">
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="15"/>
+      <c r="AH3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="AI3" s="11"/>
-      <c r="AJ3" s="11"/>
-      <c r="AK3" s="12"/>
-      <c r="AL3" s="10" t="s">
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="15"/>
+      <c r="AL3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="AM3" s="11"/>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="12"/>
-      <c r="AP3" s="10" t="s">
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="15"/>
+      <c r="AP3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="AQ3" s="11"/>
-      <c r="AR3" s="11"/>
-      <c r="AS3" s="12"/>
-      <c r="AT3" s="10" t="s">
+      <c r="AQ3" s="14"/>
+      <c r="AR3" s="14"/>
+      <c r="AS3" s="15"/>
+      <c r="AT3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="AU3" s="11"/>
-      <c r="AV3" s="11"/>
-      <c r="AW3" s="12"/>
-      <c r="AX3" s="10" t="s">
+      <c r="AU3" s="14"/>
+      <c r="AV3" s="14"/>
+      <c r="AW3" s="15"/>
+      <c r="AX3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="AY3" s="11"/>
-      <c r="AZ3" s="11"/>
-      <c r="BA3" s="12"/>
-      <c r="BB3" s="10" t="s">
+      <c r="AY3" s="14"/>
+      <c r="AZ3" s="14"/>
+      <c r="BA3" s="15"/>
+      <c r="BB3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="BC3" s="11"/>
-      <c r="BD3" s="11"/>
-      <c r="BE3" s="12"/>
-      <c r="BF3" s="10" t="s">
+      <c r="BC3" s="14"/>
+      <c r="BD3" s="14"/>
+      <c r="BE3" s="15"/>
+      <c r="BF3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="BG3" s="11"/>
-      <c r="BH3" s="11"/>
-      <c r="BI3" s="12"/>
-      <c r="BJ3" s="10" t="s">
+      <c r="BG3" s="14"/>
+      <c r="BH3" s="14"/>
+      <c r="BI3" s="15"/>
+      <c r="BJ3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="BK3" s="11"/>
-      <c r="BL3" s="11"/>
-      <c r="BM3" s="12"/>
-      <c r="BN3" s="10" t="s">
+      <c r="BK3" s="14"/>
+      <c r="BL3" s="14"/>
+      <c r="BM3" s="15"/>
+      <c r="BN3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="BO3" s="11"/>
-      <c r="BP3" s="11"/>
-      <c r="BQ3" s="12"/>
-      <c r="BR3" s="10" t="s">
+      <c r="BO3" s="14"/>
+      <c r="BP3" s="14"/>
+      <c r="BQ3" s="15"/>
+      <c r="BR3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="BS3" s="11"/>
-      <c r="BT3" s="11"/>
-      <c r="BU3" s="12"/>
-      <c r="BV3" s="10" t="s">
+      <c r="BS3" s="14"/>
+      <c r="BT3" s="14"/>
+      <c r="BU3" s="15"/>
+      <c r="BV3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="BW3" s="11"/>
-      <c r="BX3" s="11"/>
-      <c r="BY3" s="12"/>
-      <c r="BZ3" s="10" t="s">
+      <c r="BW3" s="14"/>
+      <c r="BX3" s="14"/>
+      <c r="BY3" s="15"/>
+      <c r="BZ3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="CA3" s="11"/>
-      <c r="CB3" s="11"/>
-      <c r="CC3" s="12"/>
-      <c r="CD3" s="10" t="s">
+      <c r="CA3" s="14"/>
+      <c r="CB3" s="14"/>
+      <c r="CC3" s="15"/>
+      <c r="CD3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="CE3" s="11"/>
-      <c r="CF3" s="11"/>
-      <c r="CG3" s="12"/>
-      <c r="CH3" s="10" t="s">
+      <c r="CE3" s="14"/>
+      <c r="CF3" s="14"/>
+      <c r="CG3" s="15"/>
+      <c r="CH3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="CI3" s="11"/>
-      <c r="CJ3" s="11"/>
-      <c r="CK3" s="12"/>
-      <c r="CL3" s="10" t="s">
+      <c r="CI3" s="14"/>
+      <c r="CJ3" s="14"/>
+      <c r="CK3" s="15"/>
+      <c r="CL3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="CM3" s="11"/>
-      <c r="CN3" s="11"/>
-      <c r="CO3" s="12"/>
-      <c r="CP3" s="10" t="s">
+      <c r="CM3" s="14"/>
+      <c r="CN3" s="14"/>
+      <c r="CO3" s="15"/>
+      <c r="CP3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="CQ3" s="11"/>
-      <c r="CR3" s="11"/>
-      <c r="CS3" s="12"/>
-      <c r="CT3" s="10" t="s">
+      <c r="CQ3" s="14"/>
+      <c r="CR3" s="14"/>
+      <c r="CS3" s="15"/>
+      <c r="CT3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="CU3" s="11"/>
-      <c r="CV3" s="11"/>
-      <c r="CW3" s="12"/>
-      <c r="CX3" s="10" t="s">
+      <c r="CU3" s="14"/>
+      <c r="CV3" s="14"/>
+      <c r="CW3" s="15"/>
+      <c r="CX3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="CY3" s="11"/>
-      <c r="CZ3" s="11"/>
-      <c r="DA3" s="12"/>
-      <c r="DB3" s="10" t="s">
+      <c r="CY3" s="14"/>
+      <c r="CZ3" s="14"/>
+      <c r="DA3" s="15"/>
+      <c r="DB3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="DC3" s="11"/>
-      <c r="DD3" s="11"/>
-      <c r="DE3" s="12"/>
+      <c r="DC3" s="14"/>
+      <c r="DD3" s="14"/>
+      <c r="DE3" s="15"/>
     </row>
     <row r="4" spans="1:109" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -42931,12 +42940,2404 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:DE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:Y17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:109" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="8">
+        <v>3</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="8">
+        <v>36</v>
+      </c>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="8">
+        <v>54</v>
+      </c>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="8">
+        <v>68</v>
+      </c>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="9"/>
+      <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
+      <c r="AX1" s="8">
+        <v>120</v>
+      </c>
+      <c r="AY1" s="9"/>
+      <c r="AZ1" s="9"/>
+      <c r="BA1" s="9"/>
+      <c r="BB1" s="9"/>
+      <c r="BC1" s="9"/>
+      <c r="BD1" s="9"/>
+      <c r="BE1" s="9"/>
+      <c r="BF1" s="9"/>
+      <c r="BG1" s="9"/>
+      <c r="BH1" s="9"/>
+      <c r="BI1" s="9"/>
+      <c r="BJ1" s="8">
+        <v>126</v>
+      </c>
+      <c r="BK1" s="9"/>
+      <c r="BL1" s="9"/>
+      <c r="BM1" s="9"/>
+      <c r="BN1" s="9"/>
+      <c r="BO1" s="9"/>
+      <c r="BP1" s="9"/>
+      <c r="BQ1" s="9"/>
+      <c r="BR1" s="9"/>
+      <c r="BS1" s="9"/>
+      <c r="BT1" s="9"/>
+      <c r="BU1" s="9"/>
+      <c r="BV1" s="8">
+        <v>138</v>
+      </c>
+      <c r="BW1" s="9"/>
+      <c r="BX1" s="9"/>
+      <c r="BY1" s="9"/>
+      <c r="BZ1" s="9"/>
+      <c r="CA1" s="9"/>
+      <c r="CB1" s="9"/>
+      <c r="CC1" s="9"/>
+      <c r="CD1" s="9"/>
+      <c r="CE1" s="9"/>
+      <c r="CF1" s="9"/>
+      <c r="CG1" s="9"/>
+      <c r="CH1" s="8">
+        <v>175</v>
+      </c>
+      <c r="CI1" s="9"/>
+      <c r="CJ1" s="9"/>
+      <c r="CK1" s="9"/>
+      <c r="CL1" s="9"/>
+      <c r="CM1" s="9"/>
+      <c r="CN1" s="9"/>
+      <c r="CO1" s="9"/>
+      <c r="CP1" s="9"/>
+      <c r="CQ1" s="9"/>
+      <c r="CR1" s="9"/>
+      <c r="CS1" s="9"/>
+      <c r="CT1" s="8">
+        <v>179</v>
+      </c>
+      <c r="CU1" s="9"/>
+      <c r="CV1" s="9"/>
+      <c r="CW1" s="9"/>
+      <c r="CX1" s="9"/>
+      <c r="CY1" s="9"/>
+      <c r="CZ1" s="9"/>
+      <c r="DA1" s="9"/>
+      <c r="DB1" s="9"/>
+      <c r="DC1" s="9"/>
+      <c r="DD1" s="9"/>
+      <c r="DE1" s="9"/>
+    </row>
+    <row r="2" spans="1:109" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="10">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="10">
+        <v>2</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="10">
+        <v>3</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="10">
+        <v>1</v>
+      </c>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="10">
+        <v>2</v>
+      </c>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="10">
+        <v>3</v>
+      </c>
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="10">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="11"/>
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="10">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="10">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="10">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="11"/>
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="10">
+        <v>2</v>
+      </c>
+      <c r="AQ2" s="11"/>
+      <c r="AR2" s="11"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="10">
+        <v>3</v>
+      </c>
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="11"/>
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="10">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="11"/>
+      <c r="AZ2" s="11"/>
+      <c r="BA2" s="11"/>
+      <c r="BB2" s="10">
+        <v>2</v>
+      </c>
+      <c r="BC2" s="11"/>
+      <c r="BD2" s="11"/>
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="10">
+        <v>3</v>
+      </c>
+      <c r="BG2" s="11"/>
+      <c r="BH2" s="11"/>
+      <c r="BI2" s="12"/>
+      <c r="BJ2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BK2" s="11"/>
+      <c r="BL2" s="11"/>
+      <c r="BM2" s="11"/>
+      <c r="BN2" s="10">
+        <v>2</v>
+      </c>
+      <c r="BO2" s="11"/>
+      <c r="BP2" s="11"/>
+      <c r="BQ2" s="12"/>
+      <c r="BR2" s="10">
+        <v>3</v>
+      </c>
+      <c r="BS2" s="11"/>
+      <c r="BT2" s="11"/>
+      <c r="BU2" s="12"/>
+      <c r="BV2" s="10">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="11"/>
+      <c r="BX2" s="11"/>
+      <c r="BY2" s="11"/>
+      <c r="BZ2" s="10">
+        <v>2</v>
+      </c>
+      <c r="CA2" s="11"/>
+      <c r="CB2" s="11"/>
+      <c r="CC2" s="12"/>
+      <c r="CD2" s="10">
+        <v>3</v>
+      </c>
+      <c r="CE2" s="11"/>
+      <c r="CF2" s="11"/>
+      <c r="CG2" s="12"/>
+      <c r="CH2" s="10">
+        <v>1</v>
+      </c>
+      <c r="CI2" s="11"/>
+      <c r="CJ2" s="11"/>
+      <c r="CK2" s="11"/>
+      <c r="CL2" s="10">
+        <v>2</v>
+      </c>
+      <c r="CM2" s="11"/>
+      <c r="CN2" s="11"/>
+      <c r="CO2" s="12"/>
+      <c r="CP2" s="10">
+        <v>3</v>
+      </c>
+      <c r="CQ2" s="11"/>
+      <c r="CR2" s="11"/>
+      <c r="CS2" s="12"/>
+      <c r="CT2" s="10">
+        <v>1</v>
+      </c>
+      <c r="CU2" s="11"/>
+      <c r="CV2" s="11"/>
+      <c r="CW2" s="11"/>
+      <c r="CX2" s="10">
+        <v>2</v>
+      </c>
+      <c r="CY2" s="11"/>
+      <c r="CZ2" s="11"/>
+      <c r="DA2" s="12"/>
+      <c r="DB2" s="10">
+        <v>3</v>
+      </c>
+      <c r="DC2" s="11"/>
+      <c r="DD2" s="11"/>
+      <c r="DE2" s="12"/>
+    </row>
+    <row r="3" spans="1:109" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="15"/>
+      <c r="Z3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="15"/>
+      <c r="AD3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="15"/>
+      <c r="AH3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="15"/>
+      <c r="AL3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="15"/>
+      <c r="AP3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="14"/>
+      <c r="AR3" s="14"/>
+      <c r="AS3" s="15"/>
+      <c r="AT3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="14"/>
+      <c r="AV3" s="14"/>
+      <c r="AW3" s="15"/>
+      <c r="AX3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="14"/>
+      <c r="AZ3" s="14"/>
+      <c r="BA3" s="15"/>
+      <c r="BB3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="14"/>
+      <c r="BD3" s="14"/>
+      <c r="BE3" s="15"/>
+      <c r="BF3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="14"/>
+      <c r="BH3" s="14"/>
+      <c r="BI3" s="15"/>
+      <c r="BJ3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="BK3" s="14"/>
+      <c r="BL3" s="14"/>
+      <c r="BM3" s="15"/>
+      <c r="BN3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="BO3" s="14"/>
+      <c r="BP3" s="14"/>
+      <c r="BQ3" s="15"/>
+      <c r="BR3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="BS3" s="14"/>
+      <c r="BT3" s="14"/>
+      <c r="BU3" s="15"/>
+      <c r="BV3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="BW3" s="14"/>
+      <c r="BX3" s="14"/>
+      <c r="BY3" s="15"/>
+      <c r="BZ3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="CA3" s="14"/>
+      <c r="CB3" s="14"/>
+      <c r="CC3" s="15"/>
+      <c r="CD3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="CE3" s="14"/>
+      <c r="CF3" s="14"/>
+      <c r="CG3" s="15"/>
+      <c r="CH3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="CI3" s="14"/>
+      <c r="CJ3" s="14"/>
+      <c r="CK3" s="15"/>
+      <c r="CL3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="CM3" s="14"/>
+      <c r="CN3" s="14"/>
+      <c r="CO3" s="15"/>
+      <c r="CP3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="CQ3" s="14"/>
+      <c r="CR3" s="14"/>
+      <c r="CS3" s="15"/>
+      <c r="CT3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="CU3" s="14"/>
+      <c r="CV3" s="14"/>
+      <c r="CW3" s="15"/>
+      <c r="CX3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="CY3" s="14"/>
+      <c r="CZ3" s="14"/>
+      <c r="DA3" s="15"/>
+      <c r="DB3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="DC3" s="14"/>
+      <c r="DD3" s="14"/>
+      <c r="DE3" s="15"/>
+    </row>
+    <row r="4" spans="1:109" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AP4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AT4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AV4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AW4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AZ4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BA4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BB4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BC4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="BD4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BE4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BF4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BG4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="BH4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BI4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BJ4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BK4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="BL4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BM4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BN4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BO4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="BP4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BQ4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BR4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BS4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="BT4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BU4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BV4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="BW4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="BX4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="BY4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="BZ4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="CA4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="CB4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="CC4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="CD4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="CE4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="CF4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="CG4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="CH4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="CI4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="CJ4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="CK4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="CL4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="CM4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="CN4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="CO4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="CP4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="CQ4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="CR4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="CS4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="CT4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="CU4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="CV4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="CW4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="CX4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="CY4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="CZ4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="DA4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="DB4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="DC4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="DD4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="DE4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f>AVERAGE(Dataset!B126:B130)</f>
+        <v>3553.5598</v>
+      </c>
+      <c r="C5" s="1">
+        <f>AVERAGE(Dataset!C126:C130)</f>
+        <v>45.200979469118863</v>
+      </c>
+      <c r="D5" s="1">
+        <f>AVERAGE(Dataset!D126:D130)</f>
+        <v>36.109372617026288</v>
+      </c>
+      <c r="E5" s="1">
+        <f>AVERAGE(Dataset!E126:E130)</f>
+        <v>1.6725850047042534</v>
+      </c>
+      <c r="F5" s="1">
+        <f>AVERAGE(Dataset!F126:F130)</f>
+        <v>3556.3474000000001</v>
+      </c>
+      <c r="G5" s="1">
+        <f>AVERAGE(Dataset!G126:G130)</f>
+        <v>44.253831959634773</v>
+      </c>
+      <c r="H5" s="1">
+        <f>AVERAGE(Dataset!H126:H130)</f>
+        <v>25.742534161674541</v>
+      </c>
+      <c r="I5" s="1">
+        <f>AVERAGE(Dataset!I126:I130)</f>
+        <v>1.852905500961068</v>
+      </c>
+      <c r="J5" s="1">
+        <f>AVERAGE(Dataset!J126:J130)</f>
+        <v>3567.0082000000002</v>
+      </c>
+      <c r="K5" s="1">
+        <f>AVERAGE(Dataset!K126:K130)</f>
+        <v>46.036894851504023</v>
+      </c>
+      <c r="L5" s="1">
+        <f>AVERAGE(Dataset!L126:L130)</f>
+        <v>24.170600609410677</v>
+      </c>
+      <c r="M5" s="1">
+        <f>AVERAGE(Dataset!M126:M130)</f>
+        <v>1.7943169087447717</v>
+      </c>
+      <c r="N5" s="1">
+        <f>AVERAGE(Dataset!N126:N130)</f>
+        <v>3553.2565999999997</v>
+      </c>
+      <c r="O5" s="1">
+        <f>AVERAGE(Dataset!O126:O130)</f>
+        <v>58.161860102718165</v>
+      </c>
+      <c r="P5" s="1">
+        <f>AVERAGE(Dataset!P126:P130)</f>
+        <v>39.595647324521288</v>
+      </c>
+      <c r="Q5" s="1">
+        <f>AVERAGE(Dataset!Q126:Q130)</f>
+        <v>1.2318419720808045</v>
+      </c>
+      <c r="R5" s="1">
+        <f>AVERAGE(Dataset!R126:R130)</f>
+        <v>3556.1566000000007</v>
+      </c>
+      <c r="S5" s="1">
+        <f>AVERAGE(Dataset!S126:S130)</f>
+        <v>54.459875531101659</v>
+      </c>
+      <c r="T5" s="1">
+        <f>AVERAGE(Dataset!T126:T130)</f>
+        <v>30.498218242886299</v>
+      </c>
+      <c r="U5" s="1">
+        <f>AVERAGE(Dataset!U126:U130)</f>
+        <v>1.3153718827291545</v>
+      </c>
+      <c r="V5" s="1">
+        <f>AVERAGE(Dataset!V126:V130)</f>
+        <v>3566.8165999999997</v>
+      </c>
+      <c r="W5" s="1">
+        <f>AVERAGE(Dataset!W126:W130)</f>
+        <v>53.357919427982168</v>
+      </c>
+      <c r="X5" s="1">
+        <f>AVERAGE(Dataset!X126:X130)</f>
+        <v>40.294535634070343</v>
+      </c>
+      <c r="Y5" s="1">
+        <f>AVERAGE(Dataset!Y126:Y130)</f>
+        <v>1.2299315324103297</v>
+      </c>
+      <c r="Z5" s="1">
+        <f>AVERAGE(Dataset!Z126:Z130)</f>
+        <v>3553.1902</v>
+      </c>
+      <c r="AA5" s="1">
+        <f>AVERAGE(Dataset!AA126:AA130)</f>
+        <v>28.00717185534678</v>
+      </c>
+      <c r="AB5" s="1">
+        <f>AVERAGE(Dataset!AB126:AB130)</f>
+        <v>31.26421211666942</v>
+      </c>
+      <c r="AC5" s="1">
+        <f>AVERAGE(Dataset!AC126:AC130)</f>
+        <v>1.3148832217045419</v>
+      </c>
+      <c r="AD5" s="1">
+        <f>AVERAGE(Dataset!AD126:AD130)</f>
+        <v>3556.06</v>
+      </c>
+      <c r="AE5" s="1">
+        <f>AVERAGE(Dataset!AE126:AE130)</f>
+        <v>24.022556445282309</v>
+      </c>
+      <c r="AF5" s="1">
+        <f>AVERAGE(Dataset!AF126:AF130)</f>
+        <v>22.573370162861071</v>
+      </c>
+      <c r="AG5" s="1">
+        <f>AVERAGE(Dataset!AG126:AG130)</f>
+        <v>1.3210251316000756</v>
+      </c>
+      <c r="AH5" s="1">
+        <f>AVERAGE(Dataset!AH126:AH130)</f>
+        <v>3566.6966000000002</v>
+      </c>
+      <c r="AI5" s="1">
+        <f>AVERAGE(Dataset!AI126:AI130)</f>
+        <v>26.039865189977554</v>
+      </c>
+      <c r="AJ5" s="1">
+        <f>AVERAGE(Dataset!AJ126:AJ130)</f>
+        <v>28.674131514497951</v>
+      </c>
+      <c r="AK5" s="1">
+        <f>AVERAGE(Dataset!AK126:AK130)</f>
+        <v>1.4757128656335561</v>
+      </c>
+      <c r="AL5" s="1">
+        <f>AVERAGE(Dataset!AL126:AL130)</f>
+        <v>3556.2378000000003</v>
+      </c>
+      <c r="AM5" s="1">
+        <f>AVERAGE(Dataset!AM126:AM130)</f>
+        <v>24.534259194051582</v>
+      </c>
+      <c r="AN5" s="1">
+        <f>AVERAGE(Dataset!AN126:AN130)</f>
+        <v>31.377909243594114</v>
+      </c>
+      <c r="AO5" s="1">
+        <f>AVERAGE(Dataset!AO126:AO130)</f>
+        <v>1.6844504953368375</v>
+      </c>
+      <c r="AP5" s="1">
+        <f>AVERAGE(Dataset!AP126:AP130)</f>
+        <v>3555.1258000000003</v>
+      </c>
+      <c r="AQ5" s="1">
+        <f>AVERAGE(Dataset!AQ126:AQ130)</f>
+        <v>23.764558495311324</v>
+      </c>
+      <c r="AR5" s="1">
+        <f>AVERAGE(Dataset!AR126:AR130)</f>
+        <v>17.195916893496182</v>
+      </c>
+      <c r="AS5" s="1">
+        <f>AVERAGE(Dataset!AS126:AS130)</f>
+        <v>1.6507383514000407</v>
+      </c>
+      <c r="AT5" s="1">
+        <f>AVERAGE(Dataset!AT126:AT130)</f>
+        <v>3527.3346000000006</v>
+      </c>
+      <c r="AU5" s="1">
+        <f>AVERAGE(Dataset!AU126:AU130)</f>
+        <v>25.913842241933633</v>
+      </c>
+      <c r="AV5" s="1">
+        <f>AVERAGE(Dataset!AV126:AV130)</f>
+        <v>25.081431712556288</v>
+      </c>
+      <c r="AW5" s="1">
+        <f>AVERAGE(Dataset!AW126:AW130)</f>
+        <v>1.6151805248388953</v>
+      </c>
+      <c r="AX5" s="1">
+        <f>AVERAGE(Dataset!AX126:AX130)</f>
+        <v>3546.1423999999997</v>
+      </c>
+      <c r="AY5" s="1">
+        <f>AVERAGE(Dataset!AY126:AY130)</f>
+        <v>22.51988619226718</v>
+      </c>
+      <c r="AZ5" s="1">
+        <f>AVERAGE(Dataset!AZ126:AZ130)</f>
+        <v>19.768435833118488</v>
+      </c>
+      <c r="BA5" s="1">
+        <f>AVERAGE(Dataset!BA126:BA130)</f>
+        <v>4.3130719264710864</v>
+      </c>
+      <c r="BB5" s="1">
+        <f>AVERAGE(Dataset!BB126:BB130)</f>
+        <v>3564.8328000000001</v>
+      </c>
+      <c r="BC5" s="1">
+        <f>AVERAGE(Dataset!BC126:BC130)</f>
+        <v>24.261655703399537</v>
+      </c>
+      <c r="BD5" s="1">
+        <f>AVERAGE(Dataset!BD126:BD130)</f>
+        <v>22.849083937133297</v>
+      </c>
+      <c r="BE5" s="1">
+        <f>AVERAGE(Dataset!BE126:BE130)</f>
+        <v>4.1476400301343253</v>
+      </c>
+      <c r="BF5" s="1">
+        <f>AVERAGE(Dataset!BF126:BF130)</f>
+        <v>3564.7479999999996</v>
+      </c>
+      <c r="BG5" s="1">
+        <f>AVERAGE(Dataset!BG126:BG130)</f>
+        <v>53.078899584503326</v>
+      </c>
+      <c r="BH5" s="1">
+        <f>AVERAGE(Dataset!BH126:BH130)</f>
+        <v>35.563473737664275</v>
+      </c>
+      <c r="BI5" s="1">
+        <f>AVERAGE(Dataset!BI126:BI130)</f>
+        <v>3.553967174358005</v>
+      </c>
+      <c r="BJ5" s="1">
+        <f>AVERAGE(Dataset!BJ126:BJ130)</f>
+        <v>3556.3909999999996</v>
+      </c>
+      <c r="BK5" s="1">
+        <f>AVERAGE(Dataset!BK126:BK130)</f>
+        <v>53.527918530510327</v>
+      </c>
+      <c r="BL5" s="1">
+        <f>AVERAGE(Dataset!BL126:BL130)</f>
+        <v>31.629323616257874</v>
+      </c>
+      <c r="BM5" s="1">
+        <f>AVERAGE(Dataset!BM126:BM130)</f>
+        <v>5.1163069115188495</v>
+      </c>
+      <c r="BN5" s="1">
+        <f>AVERAGE(Dataset!BN126:BN130)</f>
+        <v>3554.8519999999999</v>
+      </c>
+      <c r="BO5" s="1">
+        <f>AVERAGE(Dataset!BO126:BO130)</f>
+        <v>49.232969145178757</v>
+      </c>
+      <c r="BP5" s="1">
+        <f>AVERAGE(Dataset!BP126:BP130)</f>
+        <v>15.675791429840197</v>
+      </c>
+      <c r="BQ5" s="1">
+        <f>AVERAGE(Dataset!BQ126:BQ130)</f>
+        <v>4.9954648995229105</v>
+      </c>
+      <c r="BR5" s="1">
+        <f>AVERAGE(Dataset!BR126:BR130)</f>
+        <v>3527.1951999999997</v>
+      </c>
+      <c r="BS5" s="1">
+        <f>AVERAGE(Dataset!BS126:BS130)</f>
+        <v>53.257964368169425</v>
+      </c>
+      <c r="BT5" s="1">
+        <f>AVERAGE(Dataset!BT126:BT130)</f>
+        <v>15.131514988217059</v>
+      </c>
+      <c r="BU5" s="1">
+        <f>AVERAGE(Dataset!BU126:BU130)</f>
+        <v>4.9970620291961207</v>
+      </c>
+      <c r="BV5" s="1">
+        <f>AVERAGE(Dataset!BV126:BV130)</f>
+        <v>3556.4070000000002</v>
+      </c>
+      <c r="BW5" s="1">
+        <f>AVERAGE(Dataset!BW126:BW130)</f>
+        <v>55.305005380231322</v>
+      </c>
+      <c r="BX5" s="1">
+        <f>AVERAGE(Dataset!BX126:BX130)</f>
+        <v>40.700484609117169</v>
+      </c>
+      <c r="BY5" s="1">
+        <f>AVERAGE(Dataset!BY126:BY130)</f>
+        <v>2.0637624868485753</v>
+      </c>
+      <c r="BZ5" s="1">
+        <f>AVERAGE(Dataset!BZ126:BZ130)</f>
+        <v>3554.6215999999999</v>
+      </c>
+      <c r="CA5" s="1">
+        <f>AVERAGE(Dataset!CA126:CA130)</f>
+        <v>51.833763040762548</v>
+      </c>
+      <c r="CB5" s="1">
+        <f>AVERAGE(Dataset!CB126:CB130)</f>
+        <v>28.342339065285977</v>
+      </c>
+      <c r="CC5" s="1">
+        <f>AVERAGE(Dataset!CC126:CC130)</f>
+        <v>2.1119381238806829</v>
+      </c>
+      <c r="CD5" s="1">
+        <f>AVERAGE(Dataset!CD126:CD130)</f>
+        <v>3527.0199999999995</v>
+      </c>
+      <c r="CE5" s="1">
+        <f>AVERAGE(Dataset!CE126:CE130)</f>
+        <v>54.659068046464483</v>
+      </c>
+      <c r="CF5" s="1">
+        <f>AVERAGE(Dataset!CF126:CF130)</f>
+        <v>34.866821712204612</v>
+      </c>
+      <c r="CG5" s="1">
+        <f>AVERAGE(Dataset!CG126:CG130)</f>
+        <v>2.085534076904259</v>
+      </c>
+      <c r="CH5" s="1">
+        <f>AVERAGE(Dataset!CH126:CH130)</f>
+        <v>3546.0873999999994</v>
+      </c>
+      <c r="CI5" s="1">
+        <f>AVERAGE(Dataset!CI126:CI130)</f>
+        <v>50.715320978730055</v>
+      </c>
+      <c r="CJ5" s="1">
+        <f>AVERAGE(Dataset!CJ126:CJ130)</f>
+        <v>33.067553224845739</v>
+      </c>
+      <c r="CK5" s="1">
+        <f>AVERAGE(Dataset!CK126:CK130)</f>
+        <v>3.5593459915094732</v>
+      </c>
+      <c r="CL5" s="1">
+        <f>AVERAGE(Dataset!CL126:CL130)</f>
+        <v>3564.63</v>
+      </c>
+      <c r="CM5" s="1">
+        <f>AVERAGE(Dataset!CM126:CM130)</f>
+        <v>56.435180494109282</v>
+      </c>
+      <c r="CN5" s="1">
+        <f>AVERAGE(Dataset!CN126:CN130)</f>
+        <v>31.670511474147805</v>
+      </c>
+      <c r="CO5" s="1">
+        <f>AVERAGE(Dataset!CO126:CO130)</f>
+        <v>3.692063791308533</v>
+      </c>
+      <c r="CP5" s="1">
+        <f>AVERAGE(Dataset!CP126:CP130)</f>
+        <v>3564.6961999999999</v>
+      </c>
+      <c r="CQ5" s="1">
+        <f>AVERAGE(Dataset!CQ126:CQ130)</f>
+        <v>22.881303368247032</v>
+      </c>
+      <c r="CR5" s="1">
+        <f>AVERAGE(Dataset!CR126:CR130)</f>
+        <v>15.1484765790469</v>
+      </c>
+      <c r="CS5" s="1">
+        <f>AVERAGE(Dataset!CS126:CS130)</f>
+        <v>3.7891132659705855</v>
+      </c>
+      <c r="CT5" s="1">
+        <f>AVERAGE(Dataset!CT126:CT130)</f>
+        <v>3545.9061999999999</v>
+      </c>
+      <c r="CU5" s="1">
+        <f>AVERAGE(Dataset!CU126:CU130)</f>
+        <v>28.928586135806007</v>
+      </c>
+      <c r="CV5" s="1">
+        <f>AVERAGE(Dataset!CV126:CV130)</f>
+        <v>21.442192281923685</v>
+      </c>
+      <c r="CW5" s="1">
+        <f>AVERAGE(Dataset!CW126:CW130)</f>
+        <v>1.4186637170667551</v>
+      </c>
+      <c r="CX5" s="1">
+        <f>AVERAGE(Dataset!CX126:CX130)</f>
+        <v>3564.2538</v>
+      </c>
+      <c r="CY5" s="1">
+        <f>AVERAGE(Dataset!CY126:CY130)</f>
+        <v>27.756779793594564</v>
+      </c>
+      <c r="CZ5" s="1">
+        <f>AVERAGE(Dataset!CZ126:CZ130)</f>
+        <v>16.210686539435759</v>
+      </c>
+      <c r="DA5" s="1">
+        <f>AVERAGE(Dataset!DA126:DA130)</f>
+        <v>1.4256763123368106</v>
+      </c>
+      <c r="DB5" s="1">
+        <f>AVERAGE(Dataset!DB126:DB130)</f>
+        <v>3564.6822000000002</v>
+      </c>
+      <c r="DC5" s="1">
+        <f>AVERAGE(Dataset!DC126:DC130)</f>
+        <v>26.841751332061854</v>
+      </c>
+      <c r="DD5" s="1">
+        <f>AVERAGE(Dataset!DD126:DD130)</f>
+        <v>23.567023083422516</v>
+      </c>
+      <c r="DE5" s="1">
+        <f>AVERAGE(Dataset!DE126:DE130)</f>
+        <v>1.3723769759404336</v>
+      </c>
+    </row>
+    <row r="7" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+    </row>
+    <row r="8" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <f>B2</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <f>F2</f>
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <f>J2</f>
+        <v>3</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="1"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="1"/>
+      <c r="BC8" s="1"/>
+      <c r="BD8" s="1"/>
+      <c r="BE8" s="1"/>
+      <c r="BF8" s="1"/>
+      <c r="BG8" s="1"/>
+      <c r="BH8" s="1"/>
+      <c r="BI8" s="1"/>
+      <c r="BJ8" s="1"/>
+      <c r="BK8" s="1"/>
+      <c r="BL8" s="1"/>
+      <c r="BM8" s="1"/>
+      <c r="BN8" s="1"/>
+      <c r="BO8" s="1"/>
+      <c r="BP8" s="1"/>
+      <c r="BQ8" s="1"/>
+      <c r="BR8" s="1"/>
+      <c r="BS8" s="1"/>
+      <c r="BT8" s="1"/>
+      <c r="BU8" s="1"/>
+      <c r="BV8" s="1"/>
+      <c r="BW8" s="1"/>
+      <c r="BX8" s="1"/>
+      <c r="BY8" s="1"/>
+      <c r="BZ8" s="1"/>
+      <c r="CA8" s="1"/>
+      <c r="CB8" s="1"/>
+      <c r="CC8" s="1"/>
+      <c r="CD8" s="1"/>
+      <c r="CE8" s="1"/>
+      <c r="CF8" s="1"/>
+      <c r="CG8" s="1"/>
+      <c r="CH8" s="1"/>
+      <c r="CI8" s="1"/>
+      <c r="CJ8" s="1"/>
+      <c r="CK8" s="1"/>
+      <c r="CL8" s="1"/>
+      <c r="CM8" s="1"/>
+      <c r="CN8" s="1"/>
+      <c r="CO8" s="1"/>
+      <c r="CP8" s="1"/>
+      <c r="CQ8" s="1"/>
+      <c r="CR8" s="1"/>
+      <c r="CS8" s="1"/>
+      <c r="CT8" s="1"/>
+      <c r="CU8" s="1"/>
+      <c r="CV8" s="1"/>
+      <c r="CW8" s="1"/>
+      <c r="CX8" s="1"/>
+      <c r="CY8" s="1"/>
+      <c r="CZ8" s="1"/>
+      <c r="DA8" s="1"/>
+      <c r="DB8" s="1"/>
+      <c r="DC8" s="1"/>
+      <c r="DD8" s="1"/>
+      <c r="DE8" s="1"/>
+    </row>
+    <row r="9" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <f>B1</f>
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
+        <f>C5</f>
+        <v>45.200979469118863</v>
+      </c>
+      <c r="F9" s="1">
+        <f>G5</f>
+        <v>44.253831959634773</v>
+      </c>
+      <c r="G9" s="1">
+        <f>K5</f>
+        <v>46.036894851504023</v>
+      </c>
+      <c r="H9" s="1">
+        <f>AVERAGE(E9:G9)</f>
+        <v>45.163902093419217</v>
+      </c>
+      <c r="I9" s="1">
+        <f>STDEV(E9:G9)</f>
+        <v>0.89210950445102999</v>
+      </c>
+      <c r="J9" s="1">
+        <f>B1</f>
+        <v>3</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="1">
+        <f>D5</f>
+        <v>36.109372617026288</v>
+      </c>
+      <c r="N9" s="1">
+        <f>H5</f>
+        <v>25.742534161674541</v>
+      </c>
+      <c r="O9" s="1">
+        <f>L5</f>
+        <v>24.170600609410677</v>
+      </c>
+      <c r="P9" s="1">
+        <f>AVERAGE(M9:O9)</f>
+        <v>28.674169129370501</v>
+      </c>
+      <c r="Q9" s="1">
+        <f>STDEV(M9:O9)</f>
+        <v>6.4868661116381912</v>
+      </c>
+      <c r="R9" s="1">
+        <f>B1</f>
+        <v>3</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U9" s="1">
+        <f>E5</f>
+        <v>1.6725850047042534</v>
+      </c>
+      <c r="V9" s="1">
+        <f>I5</f>
+        <v>1.852905500961068</v>
+      </c>
+      <c r="W9" s="1">
+        <f>M5</f>
+        <v>1.7943169087447717</v>
+      </c>
+      <c r="X9" s="1">
+        <f>AVERAGE(U9:W9)</f>
+        <v>1.7732691381366976</v>
+      </c>
+      <c r="Y9" s="1">
+        <f>STDEV(U9:W9)</f>
+        <v>9.1984383610771381E-2</v>
+      </c>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="BF9" s="1"/>
+      <c r="BG9" s="1"/>
+      <c r="BH9" s="1"/>
+      <c r="BI9" s="1"/>
+      <c r="BR9" s="1"/>
+      <c r="BS9" s="1"/>
+      <c r="BT9" s="1"/>
+      <c r="BU9" s="1"/>
+      <c r="CD9" s="1"/>
+      <c r="CE9" s="1"/>
+      <c r="CF9" s="1"/>
+      <c r="CG9" s="1"/>
+      <c r="CP9" s="1"/>
+      <c r="CQ9" s="1"/>
+      <c r="CR9" s="1"/>
+      <c r="CS9" s="1"/>
+      <c r="DB9" s="1"/>
+      <c r="DC9" s="1"/>
+      <c r="DD9" s="1"/>
+      <c r="DE9" s="1"/>
+    </row>
+    <row r="10" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <f>N1</f>
+        <v>36</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1">
+        <f>O5</f>
+        <v>58.161860102718165</v>
+      </c>
+      <c r="F10" s="1">
+        <f>S5</f>
+        <v>54.459875531101659</v>
+      </c>
+      <c r="G10" s="1">
+        <f>W5</f>
+        <v>53.357919427982168</v>
+      </c>
+      <c r="H10" s="1">
+        <f>AVERAGE(E10:G10)</f>
+        <v>55.326551687267333</v>
+      </c>
+      <c r="I10" s="1">
+        <f>STDEV(E10:G10)</f>
+        <v>2.5165069384655618</v>
+      </c>
+      <c r="J10" s="1">
+        <f>N1</f>
+        <v>36</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M10" s="1">
+        <f>P5</f>
+        <v>39.595647324521288</v>
+      </c>
+      <c r="N10" s="1">
+        <f>T5</f>
+        <v>30.498218242886299</v>
+      </c>
+      <c r="O10" s="1">
+        <f>X5</f>
+        <v>40.294535634070343</v>
+      </c>
+      <c r="P10" s="1">
+        <f>AVERAGE(M10:O10)</f>
+        <v>36.796133733825975</v>
+      </c>
+      <c r="Q10" s="1">
+        <f>STDEV(M10:O10)</f>
+        <v>5.4653376716877302</v>
+      </c>
+      <c r="R10" s="1">
+        <f>N1</f>
+        <v>36</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U10" s="1">
+        <f>Q5</f>
+        <v>1.2318419720808045</v>
+      </c>
+      <c r="V10" s="1">
+        <f>U5</f>
+        <v>1.3153718827291545</v>
+      </c>
+      <c r="W10" s="1">
+        <f>Y5</f>
+        <v>1.2299315324103297</v>
+      </c>
+      <c r="X10" s="1">
+        <f>AVERAGE(U10:W10)</f>
+        <v>1.2590484624067628</v>
+      </c>
+      <c r="Y10" s="1">
+        <f>STDEV(U10:W10)</f>
+        <v>4.8786865061645715E-2</v>
+      </c>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="BF10" s="1"/>
+      <c r="BG10" s="1"/>
+      <c r="BH10" s="1"/>
+      <c r="BI10" s="1"/>
+      <c r="BR10" s="1"/>
+      <c r="BS10" s="1"/>
+      <c r="BT10" s="1"/>
+      <c r="BU10" s="1"/>
+      <c r="CD10" s="1"/>
+      <c r="CE10" s="1"/>
+      <c r="CF10" s="1"/>
+      <c r="CG10" s="1"/>
+      <c r="CP10" s="1"/>
+      <c r="CQ10" s="1"/>
+      <c r="CR10" s="1"/>
+      <c r="CS10" s="1"/>
+      <c r="DB10" s="1"/>
+      <c r="DC10" s="1"/>
+      <c r="DD10" s="1"/>
+      <c r="DE10" s="1"/>
+    </row>
+    <row r="11" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <f>Z1</f>
+        <v>54</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="1">
+        <f>AA5</f>
+        <v>28.00717185534678</v>
+      </c>
+      <c r="F11" s="1">
+        <f>AE5</f>
+        <v>24.022556445282309</v>
+      </c>
+      <c r="G11" s="1">
+        <f>AI5</f>
+        <v>26.039865189977554</v>
+      </c>
+      <c r="H11" s="1">
+        <f>AVERAGE(E11:G11)</f>
+        <v>26.023197830202218</v>
+      </c>
+      <c r="I11" s="1">
+        <f>STDEV(E11:G11)</f>
+        <v>1.992359993121781</v>
+      </c>
+      <c r="J11" s="1">
+        <f>Z1</f>
+        <v>54</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" s="1">
+        <f>AB5</f>
+        <v>31.26421211666942</v>
+      </c>
+      <c r="N11" s="1">
+        <f>AF5</f>
+        <v>22.573370162861071</v>
+      </c>
+      <c r="O11" s="1">
+        <f>AJ5</f>
+        <v>28.674131514497951</v>
+      </c>
+      <c r="P11" s="1">
+        <f>AVERAGE(M11:O11)</f>
+        <v>27.503904598009484</v>
+      </c>
+      <c r="Q11" s="1">
+        <f>STDEV(M11:O11)</f>
+        <v>4.4620350450858446</v>
+      </c>
+      <c r="R11" s="1">
+        <f>Z1</f>
+        <v>54</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U11" s="1">
+        <f>AC5</f>
+        <v>1.3148832217045419</v>
+      </c>
+      <c r="V11" s="1">
+        <f>AG5</f>
+        <v>1.3210251316000756</v>
+      </c>
+      <c r="W11" s="1">
+        <f>AK5</f>
+        <v>1.4757128656335561</v>
+      </c>
+      <c r="X11" s="1">
+        <f>AVERAGE(U11:W11)</f>
+        <v>1.3705404063127247</v>
+      </c>
+      <c r="Y11" s="1">
+        <f>STDEV(U11:W11)</f>
+        <v>9.113377756894088E-2</v>
+      </c>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="BF11" s="1"/>
+      <c r="BG11" s="1"/>
+      <c r="BH11" s="1"/>
+      <c r="BI11" s="1"/>
+      <c r="BR11" s="1"/>
+      <c r="BS11" s="1"/>
+      <c r="BT11" s="1"/>
+      <c r="BU11" s="1"/>
+      <c r="CD11" s="1"/>
+      <c r="CE11" s="1"/>
+      <c r="CF11" s="1"/>
+      <c r="CG11" s="1"/>
+      <c r="CP11" s="1"/>
+      <c r="CQ11" s="1"/>
+      <c r="CR11" s="1"/>
+      <c r="CS11" s="1"/>
+      <c r="DB11" s="1"/>
+      <c r="DC11" s="1"/>
+      <c r="DD11" s="1"/>
+      <c r="DE11" s="1"/>
+    </row>
+    <row r="12" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <f>AL1</f>
+        <v>68</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
+        <f>AM5</f>
+        <v>24.534259194051582</v>
+      </c>
+      <c r="F12" s="1">
+        <f>AQ5</f>
+        <v>23.764558495311324</v>
+      </c>
+      <c r="G12" s="1">
+        <f>AU5</f>
+        <v>25.913842241933633</v>
+      </c>
+      <c r="H12" s="1">
+        <f>AVERAGE(E12:G12)</f>
+        <v>24.73755331043218</v>
+      </c>
+      <c r="I12" s="1">
+        <f>STDEV(E12:G12)</f>
+        <v>1.0889681029258542</v>
+      </c>
+      <c r="J12" s="1">
+        <f>AL1</f>
+        <v>68</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M12" s="1">
+        <f>AN5</f>
+        <v>31.377909243594114</v>
+      </c>
+      <c r="N12" s="1">
+        <f>AR5</f>
+        <v>17.195916893496182</v>
+      </c>
+      <c r="O12" s="1">
+        <f>AV5</f>
+        <v>25.081431712556288</v>
+      </c>
+      <c r="P12" s="1">
+        <f>AVERAGE(M12:O12)</f>
+        <v>24.551752616548857</v>
+      </c>
+      <c r="Q12" s="1">
+        <f>STDEV(M12:O12)</f>
+        <v>7.1058178074814116</v>
+      </c>
+      <c r="R12" s="1">
+        <f>AL1</f>
+        <v>68</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="1">
+        <f>AO5</f>
+        <v>1.6844504953368375</v>
+      </c>
+      <c r="V12" s="1">
+        <f>AS5</f>
+        <v>1.6507383514000407</v>
+      </c>
+      <c r="W12" s="1">
+        <f>AW5</f>
+        <v>1.6151805248388953</v>
+      </c>
+      <c r="X12" s="1">
+        <f>AVERAGE(U12:W12)</f>
+        <v>1.6501231238585914</v>
+      </c>
+      <c r="Y12" s="1">
+        <f>STDEV(U12:W12)</f>
+        <v>3.4639083156057494E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <f>AX1</f>
+        <v>120</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <f>AY5</f>
+        <v>22.51988619226718</v>
+      </c>
+      <c r="F13" s="1">
+        <f>BC5</f>
+        <v>24.261655703399537</v>
+      </c>
+      <c r="G13" s="1">
+        <f>BG5</f>
+        <v>53.078899584503326</v>
+      </c>
+      <c r="H13" s="1">
+        <f>AVERAGE(E13:G13)</f>
+        <v>33.286813826723346</v>
+      </c>
+      <c r="I13" s="1">
+        <f>STDEV(E13:G13)</f>
+        <v>17.162559081907499</v>
+      </c>
+      <c r="J13" s="1">
+        <f>AX1</f>
+        <v>120</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" s="1">
+        <f>AZ5</f>
+        <v>19.768435833118488</v>
+      </c>
+      <c r="N13" s="1">
+        <f>BD5</f>
+        <v>22.849083937133297</v>
+      </c>
+      <c r="O13" s="1">
+        <f>BH5</f>
+        <v>35.563473737664275</v>
+      </c>
+      <c r="P13" s="1">
+        <f>AVERAGE(M13:O13)</f>
+        <v>26.060331169305357</v>
+      </c>
+      <c r="Q13" s="1">
+        <f>STDEV(M13:O13)</f>
+        <v>8.3728661276237357</v>
+      </c>
+      <c r="R13" s="1">
+        <f>AX1</f>
+        <v>120</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="1">
+        <f>BA5</f>
+        <v>4.3130719264710864</v>
+      </c>
+      <c r="V13" s="1">
+        <f>BE5</f>
+        <v>4.1476400301343253</v>
+      </c>
+      <c r="W13" s="1">
+        <f>BI5</f>
+        <v>3.553967174358005</v>
+      </c>
+      <c r="X13" s="1">
+        <f>AVERAGE(U13:W13)</f>
+        <v>4.0048930436544721</v>
+      </c>
+      <c r="Y13" s="1">
+        <f>STDEV(U13:W13)</f>
+        <v>0.39917731997443839</v>
+      </c>
+    </row>
+    <row r="14" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <f>BJ1</f>
+        <v>126</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1">
+        <f>BK5</f>
+        <v>53.527918530510327</v>
+      </c>
+      <c r="F14" s="1">
+        <f>BO5</f>
+        <v>49.232969145178757</v>
+      </c>
+      <c r="G14" s="1">
+        <f>BS5</f>
+        <v>53.257964368169425</v>
+      </c>
+      <c r="H14" s="1">
+        <f>AVERAGE(E14:G14)</f>
+        <v>52.006284014619496</v>
+      </c>
+      <c r="I14" s="1">
+        <f>STDEV(E14:G14)</f>
+        <v>2.4055509423492056</v>
+      </c>
+      <c r="J14" s="1">
+        <f>BJ1</f>
+        <v>126</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="1">
+        <f>BL5</f>
+        <v>31.629323616257874</v>
+      </c>
+      <c r="N14" s="1">
+        <f>BP5</f>
+        <v>15.675791429840197</v>
+      </c>
+      <c r="O14" s="1">
+        <f>BT5</f>
+        <v>15.131514988217059</v>
+      </c>
+      <c r="P14" s="1">
+        <f>AVERAGE(M14:O14)</f>
+        <v>20.812210011438378</v>
+      </c>
+      <c r="Q14" s="1">
+        <f>STDEV(M14:O14)</f>
+        <v>9.3718471640282761</v>
+      </c>
+      <c r="R14" s="1">
+        <f>BJ1</f>
+        <v>126</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" s="1">
+        <f>BM5</f>
+        <v>5.1163069115188495</v>
+      </c>
+      <c r="V14" s="1">
+        <f>BQ5</f>
+        <v>4.9954648995229105</v>
+      </c>
+      <c r="W14" s="1">
+        <f>BU5</f>
+        <v>4.9970620291961207</v>
+      </c>
+      <c r="X14" s="1">
+        <f>AVERAGE(U14:W14)</f>
+        <v>5.03627794674596</v>
+      </c>
+      <c r="Y14" s="1">
+        <f>STDEV(U14:W14)</f>
+        <v>6.9311716958704209E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <f>BV1</f>
+        <v>138</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1">
+        <f>BW5</f>
+        <v>55.305005380231322</v>
+      </c>
+      <c r="F15" s="1">
+        <f>CA5</f>
+        <v>51.833763040762548</v>
+      </c>
+      <c r="G15" s="1">
+        <f>CE5</f>
+        <v>54.659068046464483</v>
+      </c>
+      <c r="H15" s="1">
+        <f>AVERAGE(E15:G15)</f>
+        <v>53.932612155819449</v>
+      </c>
+      <c r="I15" s="1">
+        <f>STDEV(E15:G15)</f>
+        <v>1.8461268823187129</v>
+      </c>
+      <c r="J15" s="1">
+        <f>BV1</f>
+        <v>138</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" s="1">
+        <f>BX5</f>
+        <v>40.700484609117169</v>
+      </c>
+      <c r="N15" s="1">
+        <f>CB5</f>
+        <v>28.342339065285977</v>
+      </c>
+      <c r="O15" s="1">
+        <f>CF5</f>
+        <v>34.866821712204612</v>
+      </c>
+      <c r="P15" s="1">
+        <f>AVERAGE(M15:O15)</f>
+        <v>34.636548462202583</v>
+      </c>
+      <c r="Q15" s="1">
+        <f>STDEV(M15:O15)</f>
+        <v>6.1822900003056089</v>
+      </c>
+      <c r="R15" s="1">
+        <f>BV1</f>
+        <v>138</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" s="1">
+        <f>BY5</f>
+        <v>2.0637624868485753</v>
+      </c>
+      <c r="V15" s="1">
+        <f>CC5</f>
+        <v>2.1119381238806829</v>
+      </c>
+      <c r="W15" s="1">
+        <f>CG5</f>
+        <v>2.085534076904259</v>
+      </c>
+      <c r="X15" s="1">
+        <f>AVERAGE(U15:W15)</f>
+        <v>2.0870782292111723</v>
+      </c>
+      <c r="Y15" s="1">
+        <f>STDEV(U15:W15)</f>
+        <v>2.4124910479057817E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:109" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <f>CH1</f>
+        <v>175</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="1">
+        <f>CI5</f>
+        <v>50.715320978730055</v>
+      </c>
+      <c r="F16" s="1">
+        <f>CM5</f>
+        <v>56.435180494109282</v>
+      </c>
+      <c r="G16" s="1">
+        <f>CQ5</f>
+        <v>22.881303368247032</v>
+      </c>
+      <c r="H16" s="1">
+        <f>AVERAGE(E16:G16)</f>
+        <v>43.343934947028792</v>
+      </c>
+      <c r="I16" s="1">
+        <f>STDEV(E16:G16)</f>
+        <v>17.95045031651394</v>
+      </c>
+      <c r="J16" s="1">
+        <f>CH1</f>
+        <v>175</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" s="1">
+        <f>CJ5</f>
+        <v>33.067553224845739</v>
+      </c>
+      <c r="N16" s="1">
+        <f>CN5</f>
+        <v>31.670511474147805</v>
+      </c>
+      <c r="O16" s="1">
+        <f>CR5</f>
+        <v>15.1484765790469</v>
+      </c>
+      <c r="P16" s="1">
+        <f>AVERAGE(M16:O16)</f>
+        <v>26.628847092680147</v>
+      </c>
+      <c r="Q16" s="1">
+        <f>STDEV(M16:O16)</f>
+        <v>9.9668004776368999</v>
+      </c>
+      <c r="R16" s="1">
+        <f>CH1</f>
+        <v>175</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" s="1">
+        <f>CK5</f>
+        <v>3.5593459915094732</v>
+      </c>
+      <c r="V16" s="1">
+        <f>CO5</f>
+        <v>3.692063791308533</v>
+      </c>
+      <c r="W16" s="1">
+        <f>CS5</f>
+        <v>3.7891132659705855</v>
+      </c>
+      <c r="X16" s="1">
+        <f>AVERAGE(U16:W16)</f>
+        <v>3.6801743495961978</v>
+      </c>
+      <c r="Y16" s="1">
+        <f>STDEV(U16:W16)</f>
+        <v>0.11534413388419588</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <f>CT1</f>
+        <v>179</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="1">
+        <f>CU5</f>
+        <v>28.928586135806007</v>
+      </c>
+      <c r="F17" s="1">
+        <f>CY5</f>
+        <v>27.756779793594564</v>
+      </c>
+      <c r="G17" s="1">
+        <f>DC5</f>
+        <v>26.841751332061854</v>
+      </c>
+      <c r="H17" s="1">
+        <f>AVERAGE(E17:G17)</f>
+        <v>27.842372420487475</v>
+      </c>
+      <c r="I17" s="1">
+        <f>STDEV(E17:G17)</f>
+        <v>1.0460470581495349</v>
+      </c>
+      <c r="J17" s="1">
+        <f>CT1</f>
+        <v>179</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" s="1">
+        <f>CV5</f>
+        <v>21.442192281923685</v>
+      </c>
+      <c r="N17" s="1">
+        <f>CZ5</f>
+        <v>16.210686539435759</v>
+      </c>
+      <c r="O17" s="1">
+        <f>DD5</f>
+        <v>23.567023083422516</v>
+      </c>
+      <c r="P17" s="1">
+        <f>AVERAGE(M17:O17)</f>
+        <v>20.406633968260653</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>STDEV(M17:O17)</f>
+        <v>3.785922292235564</v>
+      </c>
+      <c r="R17" s="1">
+        <f>CT1</f>
+        <v>179</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U17" s="1">
+        <f>CW5</f>
+        <v>1.4186637170667551</v>
+      </c>
+      <c r="V17" s="1">
+        <f>DA5</f>
+        <v>1.4256763123368106</v>
+      </c>
+      <c r="W17" s="1">
+        <f>DE5</f>
+        <v>1.3723769759404336</v>
+      </c>
+      <c r="X17" s="1">
+        <f>AVERAGE(U17:W17)</f>
+        <v>1.4055723351146663</v>
+      </c>
+      <c r="Y17" s="1">
+        <f>STDEV(U17:W17)</f>
+        <v>2.896106051468321E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+    </row>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="63">
+    <mergeCell ref="BV1:CG1"/>
+    <mergeCell ref="CH1:CS1"/>
+    <mergeCell ref="CT1:DE1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="J2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="Z2:AC2"/>
+    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="N1:Y1"/>
+    <mergeCell ref="Z1:AK1"/>
+    <mergeCell ref="AL1:AW1"/>
+    <mergeCell ref="AX1:BI1"/>
+    <mergeCell ref="BJ1:BU1"/>
+    <mergeCell ref="BV2:BY2"/>
+    <mergeCell ref="AD2:AG2"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="AL2:AO2"/>
+    <mergeCell ref="AP2:AS2"/>
+    <mergeCell ref="AT2:AW2"/>
+    <mergeCell ref="AX2:BA2"/>
+    <mergeCell ref="BB2:BE2"/>
+    <mergeCell ref="BF2:BI2"/>
+    <mergeCell ref="BJ2:BM2"/>
+    <mergeCell ref="BN2:BQ2"/>
+    <mergeCell ref="BR2:BU2"/>
+    <mergeCell ref="CX2:DA2"/>
+    <mergeCell ref="DB2:DE2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="BZ2:CC2"/>
+    <mergeCell ref="CD2:CG2"/>
+    <mergeCell ref="CH2:CK2"/>
+    <mergeCell ref="CL2:CO2"/>
+    <mergeCell ref="CP2:CS2"/>
+    <mergeCell ref="CT2:CW2"/>
+    <mergeCell ref="BZ3:CC3"/>
+    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="AL3:AO3"/>
+    <mergeCell ref="AP3:AS3"/>
+    <mergeCell ref="AT3:AW3"/>
+    <mergeCell ref="AX3:BA3"/>
+    <mergeCell ref="BB3:BE3"/>
+    <mergeCell ref="BF3:BI3"/>
+    <mergeCell ref="BJ3:BM3"/>
+    <mergeCell ref="BN3:BQ3"/>
+    <mergeCell ref="BR3:BU3"/>
+    <mergeCell ref="BV3:BY3"/>
+    <mergeCell ref="DB3:DE3"/>
+    <mergeCell ref="CD3:CG3"/>
+    <mergeCell ref="CH3:CK3"/>
+    <mergeCell ref="CL3:CO3"/>
+    <mergeCell ref="CP3:CS3"/>
+    <mergeCell ref="CT3:CW3"/>
+    <mergeCell ref="CX3:DA3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>